<commit_message>
cambios para cargar al excel los requests
</commit_message>
<xml_diff>
--- a/IProyectoDiseño/IProyectoDiseño/src/files/DatosFormulario.xlsx
+++ b/IProyectoDiseño/IProyectoDiseño/src/files/DatosFormulario.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ersolano\OneDrive\Diseño de SW\Proyecto 1\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="24">
   <si>
     <t>Periodo</t>
   </si>
@@ -84,12 +84,27 @@
   </si>
   <si>
     <t>Me pusieron un 70 cuando lo correcto era un 75, porque al final de me dio un 72.51</t>
+  </si>
+  <si>
+    <t>2011123456</t>
+  </si>
+  <si>
+    <t>89999999</t>
+  </si>
+  <si>
+    <t>2015567890</t>
+  </si>
+  <si>
+    <t>59999999</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="d/m/yy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,10 +143,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -421,15 +492,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="6.796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="67.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.19921875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.59765625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.796875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.19921875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.59765625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="67.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
@@ -464,21 +535,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" s="1">
-        <v>42789</v>
-      </c>
-      <c r="B2">
-        <v>2011123456</v>
+    <row r="2">
+      <c r="A2" t="n" s="55">
+        <v>736858.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2">
-        <v>89999999</v>
+      <c r="E2" t="s">
+        <v>21</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -486,8 +557,8 @@
       <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="H2">
-        <v>1</v>
+      <c r="H2" t="n">
+        <v>1.0</v>
       </c>
       <c r="I2" t="s">
         <v>14</v>
@@ -496,21 +567,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
-        <v>42825</v>
-      </c>
-      <c r="B3">
-        <v>2015567890</v>
+    <row r="3">
+      <c r="A3" t="n" s="57">
+        <v>736858.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="E3">
-        <v>59999999</v>
+      <c r="E3" t="s">
+        <v>23</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -518,8 +589,8 @@
       <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="H3">
-        <v>1</v>
+      <c r="H3" t="n">
+        <v>1.0</v>
       </c>
       <c r="I3" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
tira el excel de resolution f
falta q lo lea (las resoluciones), y que al final de tirar los requests tenga el num de resolucion 
ahora en ingles lo hago :v
</commit_message>
<xml_diff>
--- a/IProyectoDiseño/IProyectoDiseño/src/files/DatosFormulario.xlsx
+++ b/IProyectoDiseño/IProyectoDiseño/src/files/DatosFormulario.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ersolano\OneDrive\Diseño de SW\Proyecto 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ariana\OneDrive\Estudiantil\Materia\2017\Diseño\Proyectos\IProyectoDiseno\IProyectoDiseño\IProyectoDiseño\src\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7433"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7428"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
   <si>
     <t>Periodo</t>
   </si>
@@ -114,14 +114,38 @@
   </si>
   <si>
     <t>hjgckgsdakvg</t>
+  </si>
+  <si>
+    <t>Id solicitante</t>
+  </si>
+  <si>
+    <t>Estado de solicitud</t>
+  </si>
+  <si>
+    <t>PENDIENTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ana maria </t>
+  </si>
+  <si>
+    <t>Nombre solicitante</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>PROCESADA</t>
+  </si>
+  <si>
+    <t>CANCELADO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="d/m/yy"/>
+    <numFmt numFmtId="164" formatCode="d/m/yy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -134,7 +158,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,79 +181,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -508,26 +476,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.19921875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.59765625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.21875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.5546875" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.796875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.19921875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.59765625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.21875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.5546875" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="67.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -558,10 +526,19 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="59">
-        <v>736858.0</v>
+      <c r="A2" t="n" s="5">
+        <v>42859.0</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -590,10 +567,19 @@
       <c r="J2" t="s">
         <v>15</v>
       </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="61">
-        <v>736858.0</v>
+      <c r="A3" t="n" s="7">
+        <v>42898.0</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -622,10 +608,19 @@
       <c r="J3" t="s">
         <v>19</v>
       </c>
+      <c r="K3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="63">
-        <v>736858.0</v>
+      <c r="A4" t="n" s="9">
+        <v>42810.0</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -654,6 +649,18 @@
       <c r="J4" t="s">
         <v>29</v>
       </c>
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -661,5 +668,6 @@
     <hyperlink ref="D3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ya guarda y carga resoluciones! :D
</commit_message>
<xml_diff>
--- a/IProyectoDiseño/IProyectoDiseño/src/files/DatosFormulario.xlsx
+++ b/IProyectoDiseño/IProyectoDiseño/src/files/DatosFormulario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="40">
   <si>
     <t>Periodo</t>
   </si>
@@ -134,10 +134,16 @@
     <t>123</t>
   </si>
   <si>
+    <t>CANCELADO</t>
+  </si>
+  <si>
+    <t>Num de Resolucion</t>
+  </si>
+  <si>
     <t>PROCESADA</t>
   </si>
   <si>
-    <t>CANCELADO</t>
+    <t>65</t>
   </si>
 </sst>
 </file>
@@ -184,12 +190,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -476,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,9 +505,11 @@
     <col min="8" max="8" bestFit="true" customWidth="true" width="5.5546875" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="67.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="19.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="16.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -535,9 +549,12 @@
       <c r="M1" t="s">
         <v>31</v>
       </c>
+      <c r="N1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="5">
+      <c r="A2" t="n" s="11">
         <v>42859.0</v>
       </c>
       <c r="B2" t="s">
@@ -574,11 +591,14 @@
         <v>33</v>
       </c>
       <c r="M2" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="N2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="7">
+      <c r="A3" t="n" s="13">
         <v>42898.0</v>
       </c>
       <c r="B3" t="s">
@@ -615,11 +635,11 @@
         <v>33</v>
       </c>
       <c r="M3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="9">
+      <c r="A4" t="n" s="15">
         <v>42810.0</v>
       </c>
       <c r="B4" t="s">
@@ -656,10 +676,10 @@
         <v>33</v>
       </c>
       <c r="M4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M5" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
No se quedo residuo
</commit_message>
<xml_diff>
--- a/IProyectoDiseño/IProyectoDiseño/src/files/DatosFormulario.xlsx
+++ b/IProyectoDiseño/IProyectoDiseño/src/files/DatosFormulario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="38">
   <si>
     <t>Periodo</t>
   </si>
@@ -185,10 +185,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -652,7 +658,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="115">
+      <c r="A2" t="n" s="121">
         <v>42789.0</v>
       </c>
       <c r="B2" t="s">
@@ -691,7 +697,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="117">
+      <c r="A3" t="n" s="123">
         <v>42825.0</v>
       </c>
       <c r="B3" t="s">
@@ -730,7 +736,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="119">
+      <c r="A4" t="n" s="125">
         <v>43285.95474537037</v>
       </c>
       <c r="B4" t="s">

</xml_diff>